<commit_message>
completing testing for phe_sii
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_SII.xlsx
+++ b/tests/testthat/testdata_SII.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emma.clegg\Documents\PHEindicatormethods\tests\testthat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{05381CB5-0ECB-4537-A9A2-DEB933F9C8FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="78" windowWidth="21078" windowHeight="10548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_SII" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="179017" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -142,7 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -501,20 +507,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Comma 2" xfId="2"/>
-    <cellStyle name="Comma 3" xfId="3"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 5" xfId="5"/>
-    <cellStyle name="Percent 2" xfId="6"/>
-    <cellStyle name="Percent 3" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Percent 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Percent 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -563,7 +572,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,9 +605,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -631,6 +657,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -806,35 +849,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F114" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R130" sqref="R130"/>
+      <selection pane="bottomRight" activeCell="R118" sqref="R118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.26171875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="47.15625" style="6" customWidth="1"/>
     <col min="3" max="3" width="13" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="61" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.7109375" style="62" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="63" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="63" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="63" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="64" customWidth="1"/>
-    <col min="14" max="21" width="12.7109375" style="6" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="12.41796875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="10.68359375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.68359375" style="62" customWidth="1"/>
+    <col min="9" max="9" width="12.68359375" style="63" customWidth="1"/>
+    <col min="10" max="10" width="12.68359375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="11.578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.41796875" style="63" customWidth="1"/>
+    <col min="13" max="13" width="12.68359375" style="64" customWidth="1"/>
+    <col min="14" max="21" width="12.68359375" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="9.15625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,13 +927,13 @@
         <v>15</v>
       </c>
       <c r="Q1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>19</v>
@@ -899,7 +942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -947,13 +990,13 @@
         <v>6.9346164736688189</v>
       </c>
       <c r="Q2" s="7">
+        <v>1.0888180804446217</v>
+      </c>
+      <c r="R2" s="7">
         <v>3.1275946176508169</v>
       </c>
-      <c r="R2" s="7">
+      <c r="S2" s="7">
         <v>10.7586873680794</v>
-      </c>
-      <c r="S2" s="7">
-        <v>1.0888180804446217</v>
       </c>
       <c r="T2" s="7">
         <v>1.0383690591642838</v>
@@ -962,7 +1005,7 @@
         <v>1.1412993360251238</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1013,7 +1056,7 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1064,7 +1107,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1115,7 +1158,7 @@
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1166,7 +1209,7 @@
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1217,7 +1260,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1268,7 +1311,7 @@
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1319,7 +1362,7 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1370,7 +1413,7 @@
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1421,7 +1464,7 @@
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -1469,13 +1512,13 @@
         <v>12.547846636351798</v>
       </c>
       <c r="Q12" s="12">
+        <v>1.180885620848795</v>
+      </c>
+      <c r="R12" s="12">
         <v>11.936156426792138</v>
       </c>
-      <c r="R12" s="12">
+      <c r="S12" s="12">
         <v>13.163020132396579</v>
-      </c>
-      <c r="S12" s="12">
-        <v>1.180885620848795</v>
       </c>
       <c r="T12" s="12">
         <v>1.1713706914325628</v>
@@ -1484,7 +1527,7 @@
         <v>1.1904396357244886</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -1535,7 +1578,7 @@
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1586,7 +1629,7 @@
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
     </row>
-    <row r="15" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1637,7 +1680,7 @@
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
     </row>
-    <row r="16" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1688,7 +1731,7 @@
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
     </row>
-    <row r="17" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1739,7 +1782,7 @@
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
     </row>
-    <row r="18" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1790,7 +1833,7 @@
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
     </row>
-    <row r="19" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -1841,7 +1884,7 @@
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
     </row>
-    <row r="20" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -1892,7 +1935,7 @@
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
     </row>
-    <row r="21" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -1943,7 +1986,7 @@
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1991,13 +2034,13 @@
         <v>6.9346164736688189</v>
       </c>
       <c r="Q22" s="7">
+        <v>1.0888180804446217</v>
+      </c>
+      <c r="R22" s="7">
         <v>1.9243274437391116</v>
       </c>
-      <c r="R22" s="7">
+      <c r="S22" s="7">
         <v>11.99208403800279</v>
-      </c>
-      <c r="S22" s="7">
-        <v>1.0888180804446217</v>
       </c>
       <c r="T22" s="7">
         <v>1.0234148326541768</v>
@@ -2006,7 +2049,7 @@
         <v>1.1587677685047233</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -2057,7 +2100,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -2108,7 +2151,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2159,7 +2202,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2210,7 +2253,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2261,7 +2304,7 @@
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -2312,7 +2355,7 @@
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -2363,7 +2406,7 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -2414,7 +2457,7 @@
       <c r="T30" s="7"/>
       <c r="U30" s="7"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -2465,7 +2508,7 @@
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -2513,13 +2556,13 @@
         <v>12.547846636351798</v>
       </c>
       <c r="Q32" s="12">
+        <v>1.180885620848795</v>
+      </c>
+      <c r="R32" s="12">
         <v>11.743647833205888</v>
       </c>
-      <c r="R32" s="12">
+      <c r="S32" s="12">
         <v>13.347203652453951</v>
-      </c>
-      <c r="S32" s="12">
-        <v>1.180885620848795</v>
       </c>
       <c r="T32" s="12">
         <v>1.168320603472105</v>
@@ -2528,7 +2571,7 @@
         <v>1.1934312559878586</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -2579,7 +2622,7 @@
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
     </row>
-    <row r="34" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -2630,7 +2673,7 @@
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
     </row>
-    <row r="35" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="12">
         <v>34</v>
       </c>
@@ -2681,7 +2724,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -2732,7 +2775,7 @@
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
     </row>
-    <row r="37" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -2783,7 +2826,7 @@
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
     </row>
-    <row r="38" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -2834,7 +2877,7 @@
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
     </row>
-    <row r="39" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -2885,7 +2928,7 @@
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
     </row>
-    <row r="40" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -2936,7 +2979,7 @@
       <c r="T40" s="12"/>
       <c r="U40" s="12"/>
     </row>
-    <row r="41" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -2987,7 +3030,7 @@
       <c r="T41" s="12"/>
       <c r="U41" s="12"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -3035,13 +3078,13 @@
         <v>6.9346164736688189</v>
       </c>
       <c r="Q42" s="7">
+        <v>1.0888180804446217</v>
+      </c>
+      <c r="R42" s="7">
         <v>3.1421243989944716</v>
       </c>
-      <c r="R42" s="7">
+      <c r="S42" s="7">
         <v>10.805621466984828</v>
-      </c>
-      <c r="S42" s="7">
-        <v>1.0888180804446217</v>
       </c>
       <c r="T42" s="7">
         <v>1.0391386444860844</v>
@@ -3050,7 +3093,7 @@
         <v>1.1407094261348529</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -3101,7 +3144,7 @@
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -3152,7 +3195,7 @@
       <c r="T44" s="7"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -3203,7 +3246,7 @@
       <c r="T45" s="7"/>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -3254,7 +3297,7 @@
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -3305,7 +3348,7 @@
       <c r="T47" s="7"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -3356,7 +3399,7 @@
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -3407,7 +3450,7 @@
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -3458,7 +3501,7 @@
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -3509,7 +3552,7 @@
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -3557,13 +3600,13 @@
         <v>12.547846636351798</v>
       </c>
       <c r="Q52" s="12">
+        <v>1.180885620848795</v>
+      </c>
+      <c r="R52" s="12">
         <v>11.937447333014509</v>
       </c>
-      <c r="R52" s="12">
+      <c r="S52" s="12">
         <v>13.16492301413779</v>
-      </c>
-      <c r="S52" s="12">
-        <v>1.180885620848795</v>
       </c>
       <c r="T52" s="12">
         <v>1.1713692255460837</v>
@@ -3572,7 +3615,7 @@
         <v>1.1905995616725575</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A53" s="12">
         <v>52</v>
       </c>
@@ -3623,7 +3666,7 @@
       <c r="T53" s="12"/>
       <c r="U53" s="12"/>
     </row>
-    <row r="54" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -3674,7 +3717,7 @@
       <c r="T54" s="12"/>
       <c r="U54" s="12"/>
     </row>
-    <row r="55" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A55" s="12">
         <v>54</v>
       </c>
@@ -3725,7 +3768,7 @@
       <c r="T55" s="12"/>
       <c r="U55" s="12"/>
     </row>
-    <row r="56" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A56" s="12">
         <v>55</v>
       </c>
@@ -3776,7 +3819,7 @@
       <c r="T56" s="12"/>
       <c r="U56" s="12"/>
     </row>
-    <row r="57" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -3827,7 +3870,7 @@
       <c r="T57" s="12"/>
       <c r="U57" s="12"/>
     </row>
-    <row r="58" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -3878,7 +3921,7 @@
       <c r="T58" s="12"/>
       <c r="U58" s="12"/>
     </row>
-    <row r="59" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A59" s="12">
         <v>58</v>
       </c>
@@ -3929,7 +3972,7 @@
       <c r="T59" s="12"/>
       <c r="U59" s="12"/>
     </row>
-    <row r="60" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -3980,7 +4023,7 @@
       <c r="T60" s="12"/>
       <c r="U60" s="12"/>
     </row>
-    <row r="61" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -4031,7 +4074,7 @@
       <c r="T61" s="12"/>
       <c r="U61" s="12"/>
     </row>
-    <row r="62" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" s="25" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A62" s="20">
         <v>61</v>
       </c>
@@ -4078,15 +4121,15 @@
       <c r="P62" s="20">
         <v>7.9193341471008738</v>
       </c>
-      <c r="Q62" s="20"/>
+      <c r="Q62" s="20">
+        <v>1.1037116952527257</v>
+      </c>
       <c r="R62" s="20"/>
-      <c r="S62" s="20">
-        <v>1.1037116952527257</v>
-      </c>
+      <c r="S62" s="20"/>
       <c r="T62" s="20"/>
       <c r="U62" s="20"/>
     </row>
-    <row r="63" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" s="25" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A63" s="20">
         <v>62</v>
       </c>
@@ -4137,7 +4180,7 @@
       <c r="T63" s="20"/>
       <c r="U63" s="20"/>
     </row>
-    <row r="64" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" s="25" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A64" s="20">
         <v>63</v>
       </c>
@@ -4188,7 +4231,7 @@
       <c r="T64" s="20"/>
       <c r="U64" s="20"/>
     </row>
-    <row r="65" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" s="25" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A65" s="20">
         <v>64</v>
       </c>
@@ -4239,7 +4282,7 @@
       <c r="T65" s="20"/>
       <c r="U65" s="20"/>
     </row>
-    <row r="66" spans="1:21" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" s="25" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A66" s="20">
         <v>65</v>
       </c>
@@ -4290,7 +4333,7 @@
       <c r="T66" s="20"/>
       <c r="U66" s="20"/>
     </row>
-    <row r="67" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A67" s="12">
         <v>66</v>
       </c>
@@ -4337,15 +4380,15 @@
       <c r="P67" s="12">
         <v>3.6215563376545648</v>
       </c>
-      <c r="Q67" s="12"/>
+      <c r="Q67" s="12">
+        <v>1.0513892712719326</v>
+      </c>
       <c r="R67" s="12"/>
-      <c r="S67" s="12">
-        <v>1.0513892712719326</v>
-      </c>
+      <c r="S67" s="12"/>
       <c r="T67" s="12"/>
       <c r="U67" s="12"/>
     </row>
-    <row r="68" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A68" s="12">
         <v>67</v>
       </c>
@@ -4396,7 +4439,7 @@
       <c r="T68" s="12"/>
       <c r="U68" s="12"/>
     </row>
-    <row r="69" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A69" s="12">
         <v>68</v>
       </c>
@@ -4447,7 +4490,7 @@
       <c r="T69" s="12"/>
       <c r="U69" s="12"/>
     </row>
-    <row r="70" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A70" s="12">
         <v>69</v>
       </c>
@@ -4498,7 +4541,7 @@
       <c r="T70" s="12"/>
       <c r="U70" s="12"/>
     </row>
-    <row r="71" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="26">
         <v>70</v>
       </c>
@@ -4549,7 +4592,7 @@
       <c r="T71" s="26"/>
       <c r="U71" s="26"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A72" s="33">
         <v>71</v>
       </c>
@@ -4597,13 +4640,13 @@
         <v>-3.2752012326471758</v>
       </c>
       <c r="Q72" s="33">
+        <v>0.40600068953980034</v>
+      </c>
+      <c r="R72" s="33">
         <v>-3.5868233016744155</v>
       </c>
-      <c r="R72" s="33">
+      <c r="S72" s="33">
         <v>-2.9653170017272723</v>
-      </c>
-      <c r="S72" s="33">
-        <v>0.40600068953980034</v>
       </c>
       <c r="T72" s="33">
         <v>0.36888170199068804</v>
@@ -4612,7 +4655,7 @@
         <v>0.44624776652446996</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -4663,7 +4706,7 @@
       <c r="T73" s="7"/>
       <c r="U73" s="7"/>
     </row>
-    <row r="74" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -4714,7 +4757,7 @@
       <c r="T74" s="7"/>
       <c r="U74" s="7"/>
     </row>
-    <row r="75" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -4765,7 +4808,7 @@
       <c r="T75" s="7"/>
       <c r="U75" s="7"/>
     </row>
-    <row r="76" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -4816,7 +4859,7 @@
       <c r="T76" s="7"/>
       <c r="U76" s="7"/>
     </row>
-    <row r="77" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -4867,7 +4910,7 @@
       <c r="T77" s="7"/>
       <c r="U77" s="7"/>
     </row>
-    <row r="78" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -4918,7 +4961,7 @@
       <c r="T78" s="7"/>
       <c r="U78" s="7"/>
     </row>
-    <row r="79" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -4969,7 +5012,7 @@
       <c r="T79" s="7"/>
       <c r="U79" s="7"/>
     </row>
-    <row r="80" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -5020,7 +5063,7 @@
       <c r="T80" s="7"/>
       <c r="U80" s="7"/>
     </row>
-    <row r="81" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -5071,7 +5114,7 @@
       <c r="T81" s="7"/>
       <c r="U81" s="7"/>
     </row>
-    <row r="82" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A82" s="12">
         <v>81</v>
       </c>
@@ -5121,13 +5164,13 @@
         <v>-2.2876789027787421</v>
       </c>
       <c r="Q82" s="12">
+        <v>0.53525176979876143</v>
+      </c>
+      <c r="R82" s="12">
         <v>-2.3985255584029543</v>
       </c>
-      <c r="R82" s="12">
+      <c r="S82" s="12">
         <v>-2.1761883614121236</v>
-      </c>
-      <c r="S82" s="12">
-        <v>0.53525176979876143</v>
       </c>
       <c r="T82" s="12">
         <v>0.51734312584916309</v>
@@ -5136,7 +5179,7 @@
         <v>0.55373948894972824</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A83" s="12">
         <v>82</v>
       </c>
@@ -5189,7 +5232,7 @@
       <c r="T83" s="12"/>
       <c r="U83" s="12"/>
     </row>
-    <row r="84" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A84" s="12">
         <v>83</v>
       </c>
@@ -5242,7 +5285,7 @@
       <c r="T84" s="12"/>
       <c r="U84" s="12"/>
     </row>
-    <row r="85" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A85" s="12">
         <v>84</v>
       </c>
@@ -5295,7 +5338,7 @@
       <c r="T85" s="12"/>
       <c r="U85" s="12"/>
     </row>
-    <row r="86" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A86" s="12">
         <v>85</v>
       </c>
@@ -5348,7 +5391,7 @@
       <c r="T86" s="12"/>
       <c r="U86" s="12"/>
     </row>
-    <row r="87" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A87" s="12">
         <v>86</v>
       </c>
@@ -5401,7 +5444,7 @@
       <c r="T87" s="12"/>
       <c r="U87" s="12"/>
     </row>
-    <row r="88" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A88" s="12">
         <v>87</v>
       </c>
@@ -5454,7 +5497,7 @@
       <c r="T88" s="12"/>
       <c r="U88" s="12"/>
     </row>
-    <row r="89" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A89" s="12">
         <v>88</v>
       </c>
@@ -5507,7 +5550,7 @@
       <c r="T89" s="12"/>
       <c r="U89" s="12"/>
     </row>
-    <row r="90" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A90" s="12">
         <v>89</v>
       </c>
@@ -5560,7 +5603,7 @@
       <c r="T90" s="12"/>
       <c r="U90" s="12"/>
     </row>
-    <row r="91" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="26">
         <v>90</v>
       </c>
@@ -5613,7 +5656,7 @@
       <c r="T91" s="26"/>
       <c r="U91" s="26"/>
     </row>
-    <row r="92" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A92" s="33">
         <v>91</v>
       </c>
@@ -5663,13 +5706,13 @@
         <v>-0.10720032333730493</v>
       </c>
       <c r="Q92" s="33">
+        <v>0.53340153064655071</v>
+      </c>
+      <c r="R92" s="33">
         <v>-0.11220857220984691</v>
       </c>
-      <c r="R92" s="33">
+      <c r="S92" s="33">
         <v>-0.1021798062145461</v>
-      </c>
-      <c r="S92" s="33">
-        <v>0.53340153064655071</v>
       </c>
       <c r="T92" s="33">
         <v>0.51712731963580183</v>
@@ -5678,7 +5721,7 @@
         <v>0.55015384129130041</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -5731,7 +5774,7 @@
       <c r="T93" s="7"/>
       <c r="U93" s="7"/>
     </row>
-    <row r="94" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -5784,7 +5827,7 @@
       <c r="T94" s="7"/>
       <c r="U94" s="7"/>
     </row>
-    <row r="95" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -5837,7 +5880,7 @@
       <c r="T95" s="7"/>
       <c r="U95" s="7"/>
     </row>
-    <row r="96" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -5890,7 +5933,7 @@
       <c r="T96" s="7"/>
       <c r="U96" s="7"/>
     </row>
-    <row r="97" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -5943,7 +5986,7 @@
       <c r="T97" s="7"/>
       <c r="U97" s="7"/>
     </row>
-    <row r="98" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -5996,7 +6039,7 @@
       <c r="T98" s="7"/>
       <c r="U98" s="7"/>
     </row>
-    <row r="99" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -6049,7 +6092,7 @@
       <c r="T99" s="7"/>
       <c r="U99" s="7"/>
     </row>
-    <row r="100" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -6102,7 +6145,7 @@
       <c r="T100" s="7"/>
       <c r="U100" s="7"/>
     </row>
-    <row r="101" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A101" s="7">
         <v>100</v>
       </c>
@@ -6155,7 +6198,7 @@
       <c r="T101" s="7"/>
       <c r="U101" s="7"/>
     </row>
-    <row r="102" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A102" s="12">
         <v>101</v>
       </c>
@@ -6205,13 +6248,13 @@
         <v>-5.81854710713103E-2</v>
       </c>
       <c r="Q102" s="12">
+        <v>0.54701284615554346</v>
+      </c>
+      <c r="R102" s="12">
         <v>-6.2166295708858489E-2</v>
       </c>
-      <c r="R102" s="12">
+      <c r="S102" s="12">
         <v>-5.4174547731294348E-2</v>
-      </c>
-      <c r="S102" s="12">
-        <v>0.54701284615554346</v>
       </c>
       <c r="T102" s="12">
         <v>0.52371450740074543</v>
@@ -6220,7 +6263,7 @@
         <v>0.5714617043537692</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A103" s="12">
         <v>102</v>
       </c>
@@ -6273,7 +6316,7 @@
       <c r="T103" s="12"/>
       <c r="U103" s="12"/>
     </row>
-    <row r="104" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A104" s="12">
         <v>103</v>
       </c>
@@ -6326,7 +6369,7 @@
       <c r="T104" s="12"/>
       <c r="U104" s="12"/>
     </row>
-    <row r="105" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A105" s="12">
         <v>104</v>
       </c>
@@ -6379,7 +6422,7 @@
       <c r="T105" s="12"/>
       <c r="U105" s="12"/>
     </row>
-    <row r="106" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A106" s="12">
         <v>105</v>
       </c>
@@ -6432,7 +6475,7 @@
       <c r="T106" s="12"/>
       <c r="U106" s="12"/>
     </row>
-    <row r="107" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A107" s="12">
         <v>106</v>
       </c>
@@ -6485,7 +6528,7 @@
       <c r="T107" s="12"/>
       <c r="U107" s="12"/>
     </row>
-    <row r="108" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A108" s="12">
         <v>107</v>
       </c>
@@ -6538,7 +6581,7 @@
       <c r="T108" s="12"/>
       <c r="U108" s="12"/>
     </row>
-    <row r="109" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A109" s="12">
         <v>108</v>
       </c>
@@ -6591,7 +6634,7 @@
       <c r="T109" s="12"/>
       <c r="U109" s="12"/>
     </row>
-    <row r="110" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A110" s="12">
         <v>109</v>
       </c>
@@ -6644,7 +6687,7 @@
       <c r="T110" s="12"/>
       <c r="U110" s="12"/>
     </row>
-    <row r="111" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A111" s="12">
         <v>110</v>
       </c>
@@ -6697,7 +6740,7 @@
       <c r="T111" s="12"/>
       <c r="U111" s="12"/>
     </row>
-    <row r="112" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A112" s="7">
         <v>111</v>
       </c>
@@ -6748,16 +6791,16 @@
         <v>-10.720032333730494</v>
       </c>
       <c r="Q112" s="7">
-        <f t="shared" ref="Q112" si="2">Q92*100</f>
+        <f>Q92</f>
+        <v>0.53340153064655071</v>
+      </c>
+      <c r="R112" s="7">
+        <f t="shared" ref="R112" si="2">R92*100</f>
         <v>-11.220857220984691</v>
       </c>
-      <c r="R112" s="7">
-        <f>R92*100</f>
+      <c r="S112" s="7">
+        <f>S92*100</f>
         <v>-10.217980621454609</v>
-      </c>
-      <c r="S112" s="7">
-        <f>S92</f>
-        <v>0.53340153064655071</v>
       </c>
       <c r="T112" s="7">
         <f t="shared" ref="T112:U112" si="3">T92</f>
@@ -6768,7 +6811,7 @@
         <v>0.55015384129130041</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A113" s="7">
         <v>112</v>
       </c>
@@ -6821,7 +6864,7 @@
       <c r="T113" s="7"/>
       <c r="U113" s="7"/>
     </row>
-    <row r="114" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A114" s="7">
         <v>113</v>
       </c>
@@ -6874,7 +6917,7 @@
       <c r="T114" s="7"/>
       <c r="U114" s="7"/>
     </row>
-    <row r="115" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A115" s="7">
         <v>114</v>
       </c>
@@ -6927,7 +6970,7 @@
       <c r="T115" s="7"/>
       <c r="U115" s="7"/>
     </row>
-    <row r="116" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A116" s="7">
         <v>115</v>
       </c>
@@ -6980,7 +7023,7 @@
       <c r="T116" s="7"/>
       <c r="U116" s="7"/>
     </row>
-    <row r="117" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A117" s="7">
         <v>116</v>
       </c>
@@ -7033,7 +7076,7 @@
       <c r="T117" s="7"/>
       <c r="U117" s="7"/>
     </row>
-    <row r="118" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A118" s="7">
         <v>117</v>
       </c>
@@ -7086,7 +7129,7 @@
       <c r="T118" s="7"/>
       <c r="U118" s="7"/>
     </row>
-    <row r="119" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A119" s="7">
         <v>118</v>
       </c>
@@ -7139,7 +7182,7 @@
       <c r="T119" s="7"/>
       <c r="U119" s="7"/>
     </row>
-    <row r="120" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A120" s="7">
         <v>119</v>
       </c>
@@ -7192,7 +7235,7 @@
       <c r="T120" s="7"/>
       <c r="U120" s="7"/>
     </row>
-    <row r="121" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A121" s="7">
         <v>120</v>
       </c>
@@ -7245,7 +7288,7 @@
       <c r="T121" s="7"/>
       <c r="U121" s="7"/>
     </row>
-    <row r="122" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A122" s="12">
         <v>121</v>
       </c>
@@ -7296,16 +7339,16 @@
         <v>-5.81854710713103</v>
       </c>
       <c r="Q122" s="12">
-        <f t="shared" ref="Q122:R122" si="4">Q102*100</f>
+        <f>Q102</f>
+        <v>0.54701284615554346</v>
+      </c>
+      <c r="R122" s="12">
+        <f t="shared" ref="R122:S122" si="4">R102*100</f>
         <v>-6.216629570885849</v>
       </c>
-      <c r="R122" s="12">
+      <c r="S122" s="12">
         <f t="shared" si="4"/>
         <v>-5.4174547731294345</v>
-      </c>
-      <c r="S122" s="12">
-        <f>S102</f>
-        <v>0.54701284615554346</v>
       </c>
       <c r="T122" s="12">
         <f t="shared" ref="T122:U122" si="5">T102</f>
@@ -7316,7 +7359,7 @@
         <v>0.5714617043537692</v>
       </c>
     </row>
-    <row r="123" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A123" s="12">
         <v>122</v>
       </c>
@@ -7369,7 +7412,7 @@
       <c r="T123" s="12"/>
       <c r="U123" s="12"/>
     </row>
-    <row r="124" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A124" s="12">
         <v>123</v>
       </c>
@@ -7422,7 +7465,7 @@
       <c r="T124" s="12"/>
       <c r="U124" s="12"/>
     </row>
-    <row r="125" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A125" s="12">
         <v>124</v>
       </c>
@@ -7475,7 +7518,7 @@
       <c r="T125" s="12"/>
       <c r="U125" s="12"/>
     </row>
-    <row r="126" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A126" s="12">
         <v>125</v>
       </c>
@@ -7528,7 +7571,7 @@
       <c r="T126" s="12"/>
       <c r="U126" s="12"/>
     </row>
-    <row r="127" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A127" s="12">
         <v>126</v>
       </c>
@@ -7581,7 +7624,7 @@
       <c r="T127" s="12"/>
       <c r="U127" s="12"/>
     </row>
-    <row r="128" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A128" s="12">
         <v>127</v>
       </c>
@@ -7634,7 +7677,7 @@
       <c r="T128" s="12"/>
       <c r="U128" s="12"/>
     </row>
-    <row r="129" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A129" s="12">
         <v>128</v>
       </c>
@@ -7687,7 +7730,7 @@
       <c r="T129" s="12"/>
       <c r="U129" s="12"/>
     </row>
-    <row r="130" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A130" s="12">
         <v>129</v>
       </c>
@@ -7740,7 +7783,7 @@
       <c r="T130" s="12"/>
       <c r="U130" s="12"/>
     </row>
-    <row r="131" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="26">
         <v>130</v>
       </c>
@@ -7793,7 +7836,7 @@
       <c r="T131" s="26"/>
       <c r="U131" s="26"/>
     </row>
-    <row r="132" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A132" s="7">
         <v>131</v>
       </c>
@@ -7844,16 +7887,16 @@
         <v>10.720032333730494</v>
       </c>
       <c r="Q132" s="7">
+        <f>1/Q112</f>
+        <v>1.8747602744744141</v>
+      </c>
+      <c r="R132" s="7">
+        <f>-1*S112</f>
+        <v>10.217980621454609</v>
+      </c>
+      <c r="S132" s="7">
         <f>-1*R112</f>
-        <v>10.217980621454609</v>
-      </c>
-      <c r="R132" s="7">
-        <f>-1*Q112</f>
         <v>11.220857220984691</v>
-      </c>
-      <c r="S132" s="7">
-        <f>1/S112</f>
-        <v>1.8747602744744141</v>
       </c>
       <c r="T132" s="7">
         <f>1/U112</f>
@@ -7864,7 +7907,7 @@
         <v>1.9337597570831719</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A133" s="7">
         <v>132</v>
       </c>
@@ -7917,7 +7960,7 @@
       <c r="T133" s="7"/>
       <c r="U133" s="7"/>
     </row>
-    <row r="134" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A134" s="7">
         <v>133</v>
       </c>
@@ -7970,7 +8013,7 @@
       <c r="T134" s="7"/>
       <c r="U134" s="7"/>
     </row>
-    <row r="135" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A135" s="7">
         <v>134</v>
       </c>
@@ -8023,7 +8066,7 @@
       <c r="T135" s="7"/>
       <c r="U135" s="7"/>
     </row>
-    <row r="136" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A136" s="7">
         <v>135</v>
       </c>
@@ -8076,7 +8119,7 @@
       <c r="T136" s="7"/>
       <c r="U136" s="7"/>
     </row>
-    <row r="137" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A137" s="7">
         <v>136</v>
       </c>
@@ -8129,7 +8172,7 @@
       <c r="T137" s="7"/>
       <c r="U137" s="7"/>
     </row>
-    <row r="138" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A138" s="7">
         <v>137</v>
       </c>
@@ -8182,7 +8225,7 @@
       <c r="T138" s="7"/>
       <c r="U138" s="7"/>
     </row>
-    <row r="139" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A139" s="7">
         <v>138</v>
       </c>
@@ -8235,7 +8278,7 @@
       <c r="T139" s="7"/>
       <c r="U139" s="7"/>
     </row>
-    <row r="140" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A140" s="7">
         <v>139</v>
       </c>
@@ -8288,7 +8331,7 @@
       <c r="T140" s="7"/>
       <c r="U140" s="7"/>
     </row>
-    <row r="141" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A141" s="7">
         <v>140</v>
       </c>
@@ -8341,7 +8384,7 @@
       <c r="T141" s="7"/>
       <c r="U141" s="7"/>
     </row>
-    <row r="142" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A142" s="12">
         <v>141</v>
       </c>
@@ -8392,16 +8435,16 @@
         <v>5.81854710713103</v>
       </c>
       <c r="Q142" s="12">
+        <f>1/Q122</f>
+        <v>1.8281106321873277</v>
+      </c>
+      <c r="R142" s="12">
+        <f>-1*S122</f>
+        <v>5.4174547731294345</v>
+      </c>
+      <c r="S142" s="12">
         <f>-1*R122</f>
-        <v>5.4174547731294345</v>
-      </c>
-      <c r="R142" s="12">
-        <f>-1*Q122</f>
         <v>6.216629570885849</v>
-      </c>
-      <c r="S142" s="12">
-        <f>1/S122</f>
-        <v>1.8281106321873277</v>
       </c>
       <c r="T142" s="12">
         <f>1/U122</f>
@@ -8412,7 +8455,7 @@
         <v>1.909437271392602</v>
       </c>
     </row>
-    <row r="143" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A143" s="12">
         <v>142</v>
       </c>
@@ -8465,7 +8508,7 @@
       <c r="T143" s="12"/>
       <c r="U143" s="12"/>
     </row>
-    <row r="144" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A144" s="12">
         <v>143</v>
       </c>
@@ -8518,7 +8561,7 @@
       <c r="T144" s="12"/>
       <c r="U144" s="12"/>
     </row>
-    <row r="145" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A145" s="12">
         <v>144</v>
       </c>
@@ -8571,7 +8614,7 @@
       <c r="T145" s="12"/>
       <c r="U145" s="12"/>
     </row>
-    <row r="146" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A146" s="12">
         <v>145</v>
       </c>
@@ -8624,7 +8667,7 @@
       <c r="T146" s="12"/>
       <c r="U146" s="12"/>
     </row>
-    <row r="147" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A147" s="12">
         <v>146</v>
       </c>
@@ -8677,7 +8720,7 @@
       <c r="T147" s="12"/>
       <c r="U147" s="12"/>
     </row>
-    <row r="148" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A148" s="12">
         <v>147</v>
       </c>
@@ -8730,7 +8773,7 @@
       <c r="T148" s="12"/>
       <c r="U148" s="12"/>
     </row>
-    <row r="149" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A149" s="12">
         <v>148</v>
       </c>
@@ -8783,7 +8826,7 @@
       <c r="T149" s="12"/>
       <c r="U149" s="12"/>
     </row>
-    <row r="150" spans="1:21" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" s="18" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A150" s="12">
         <v>149</v>
       </c>
@@ -8836,7 +8879,7 @@
       <c r="T150" s="12"/>
       <c r="U150" s="12"/>
     </row>
-    <row r="151" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="26">
         <v>150</v>
       </c>
@@ -8889,7 +8932,7 @@
       <c r="T151" s="26"/>
       <c r="U151" s="26"/>
     </row>
-    <row r="152" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A152" s="33">
         <v>151</v>
       </c>
@@ -8942,7 +8985,7 @@
       <c r="T152" s="40"/>
       <c r="U152" s="40"/>
     </row>
-    <row r="153" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A153" s="7">
         <v>152</v>
       </c>
@@ -8995,7 +9038,7 @@
       <c r="T153" s="20"/>
       <c r="U153" s="20"/>
     </row>
-    <row r="154" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A154" s="7">
         <v>153</v>
       </c>
@@ -9048,7 +9091,7 @@
       <c r="T154" s="20"/>
       <c r="U154" s="20"/>
     </row>
-    <row r="155" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A155" s="7">
         <v>154</v>
       </c>
@@ -9101,7 +9144,7 @@
       <c r="T155" s="20"/>
       <c r="U155" s="20"/>
     </row>
-    <row r="156" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A156" s="7">
         <v>155</v>
       </c>
@@ -9154,7 +9197,7 @@
       <c r="T156" s="20"/>
       <c r="U156" s="20"/>
     </row>
-    <row r="157" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A157" s="7">
         <v>156</v>
       </c>
@@ -9207,7 +9250,7 @@
       <c r="T157" s="20"/>
       <c r="U157" s="20"/>
     </row>
-    <row r="158" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A158" s="7">
         <v>157</v>
       </c>
@@ -9260,7 +9303,7 @@
       <c r="T158" s="20"/>
       <c r="U158" s="20"/>
     </row>
-    <row r="159" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A159" s="7">
         <v>158</v>
       </c>
@@ -9313,7 +9356,7 @@
       <c r="T159" s="20"/>
       <c r="U159" s="20"/>
     </row>
-    <row r="160" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A160" s="7">
         <v>159</v>
       </c>
@@ -9366,7 +9409,7 @@
       <c r="T160" s="20"/>
       <c r="U160" s="20"/>
     </row>
-    <row r="161" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="46">
         <v>160</v>
       </c>
@@ -9419,7 +9462,7 @@
       <c r="T161" s="49"/>
       <c r="U161" s="49"/>
     </row>
-    <row r="162" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A162" s="33">
         <v>161</v>
       </c>
@@ -9472,7 +9515,7 @@
       <c r="T162" s="40"/>
       <c r="U162" s="40"/>
     </row>
-    <row r="163" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A163" s="7">
         <v>162</v>
       </c>
@@ -9525,7 +9568,7 @@
       <c r="T163" s="20"/>
       <c r="U163" s="20"/>
     </row>
-    <row r="164" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A164" s="7">
         <v>163</v>
       </c>
@@ -9578,7 +9621,7 @@
       <c r="T164" s="20"/>
       <c r="U164" s="20"/>
     </row>
-    <row r="165" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A165" s="7">
         <v>164</v>
       </c>
@@ -9631,7 +9674,7 @@
       <c r="T165" s="20"/>
       <c r="U165" s="20"/>
     </row>
-    <row r="166" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A166" s="7">
         <v>165</v>
       </c>
@@ -9684,7 +9727,7 @@
       <c r="T166" s="20"/>
       <c r="U166" s="20"/>
     </row>
-    <row r="167" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A167" s="7">
         <v>166</v>
       </c>
@@ -9737,7 +9780,7 @@
       <c r="T167" s="20"/>
       <c r="U167" s="20"/>
     </row>
-    <row r="168" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A168" s="7">
         <v>167</v>
       </c>
@@ -9790,7 +9833,7 @@
       <c r="T168" s="20"/>
       <c r="U168" s="20"/>
     </row>
-    <row r="169" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A169" s="7">
         <v>168</v>
       </c>
@@ -9843,7 +9886,7 @@
       <c r="T169" s="20"/>
       <c r="U169" s="20"/>
     </row>
-    <row r="170" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A170" s="7">
         <v>169</v>
       </c>
@@ -9896,7 +9939,7 @@
       <c r="T170" s="20"/>
       <c r="U170" s="20"/>
     </row>
-    <row r="171" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="46">
         <v>170</v>
       </c>
@@ -9949,7 +9992,7 @@
       <c r="T171" s="49"/>
       <c r="U171" s="49"/>
     </row>
-    <row r="172" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A172" s="33">
         <v>171</v>
       </c>
@@ -10002,7 +10045,7 @@
       <c r="T172" s="40"/>
       <c r="U172" s="40"/>
     </row>
-    <row r="173" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A173" s="7">
         <v>172</v>
       </c>
@@ -10055,7 +10098,7 @@
       <c r="T173" s="20"/>
       <c r="U173" s="20"/>
     </row>
-    <row r="174" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A174" s="7">
         <v>173</v>
       </c>
@@ -10108,7 +10151,7 @@
       <c r="T174" s="20"/>
       <c r="U174" s="20"/>
     </row>
-    <row r="175" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A175" s="7">
         <v>174</v>
       </c>
@@ -10161,7 +10204,7 @@
       <c r="T175" s="20"/>
       <c r="U175" s="20"/>
     </row>
-    <row r="176" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A176" s="7">
         <v>175</v>
       </c>
@@ -10214,7 +10257,7 @@
       <c r="T176" s="20"/>
       <c r="U176" s="20"/>
     </row>
-    <row r="177" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A177" s="7">
         <v>176</v>
       </c>
@@ -10267,7 +10310,7 @@
       <c r="T177" s="20"/>
       <c r="U177" s="20"/>
     </row>
-    <row r="178" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A178" s="7">
         <v>177</v>
       </c>
@@ -10320,7 +10363,7 @@
       <c r="T178" s="20"/>
       <c r="U178" s="20"/>
     </row>
-    <row r="179" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A179" s="7">
         <v>178</v>
       </c>
@@ -10373,7 +10416,7 @@
       <c r="T179" s="20"/>
       <c r="U179" s="20"/>
     </row>
-    <row r="180" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A180" s="7">
         <v>179</v>
       </c>
@@ -10426,7 +10469,7 @@
       <c r="T180" s="20"/>
       <c r="U180" s="20"/>
     </row>
-    <row r="181" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="46">
         <v>180</v>
       </c>
@@ -10479,7 +10522,7 @@
       <c r="T181" s="49"/>
       <c r="U181" s="49"/>
     </row>
-    <row r="182" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A182" s="33">
         <v>181</v>
       </c>
@@ -10530,7 +10573,7 @@
       <c r="T182" s="40"/>
       <c r="U182" s="40"/>
     </row>
-    <row r="183" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A183" s="7">
         <v>182</v>
       </c>
@@ -10581,7 +10624,7 @@
       <c r="T183" s="20"/>
       <c r="U183" s="20"/>
     </row>
-    <row r="184" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A184" s="7">
         <v>183</v>
       </c>
@@ -10632,7 +10675,7 @@
       <c r="T184" s="20"/>
       <c r="U184" s="20"/>
     </row>
-    <row r="185" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A185" s="7">
         <v>184</v>
       </c>
@@ -10683,7 +10726,7 @@
       <c r="T185" s="20"/>
       <c r="U185" s="20"/>
     </row>
-    <row r="186" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A186" s="7">
         <v>185</v>
       </c>
@@ -10734,7 +10777,7 @@
       <c r="T186" s="20"/>
       <c r="U186" s="20"/>
     </row>
-    <row r="187" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A187" s="7">
         <v>186</v>
       </c>
@@ -10785,7 +10828,7 @@
       <c r="T187" s="20"/>
       <c r="U187" s="20"/>
     </row>
-    <row r="188" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A188" s="7">
         <v>187</v>
       </c>
@@ -10836,7 +10879,7 @@
       <c r="T188" s="20"/>
       <c r="U188" s="20"/>
     </row>
-    <row r="189" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A189" s="7">
         <v>188</v>
       </c>
@@ -10887,7 +10930,7 @@
       <c r="T189" s="20"/>
       <c r="U189" s="20"/>
     </row>
-    <row r="190" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A190" s="7">
         <v>189</v>
       </c>
@@ -10938,7 +10981,7 @@
       <c r="T190" s="20"/>
       <c r="U190" s="20"/>
     </row>
-    <row r="191" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="46">
         <v>190</v>
       </c>
@@ -10989,7 +11032,7 @@
       <c r="T191" s="49"/>
       <c r="U191" s="49"/>
     </row>
-    <row r="192" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A192" s="33">
         <v>191</v>
       </c>
@@ -11036,7 +11079,7 @@
       <c r="T192" s="40"/>
       <c r="U192" s="40"/>
     </row>
-    <row r="193" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A193" s="7">
         <v>192</v>
       </c>
@@ -11083,7 +11126,7 @@
       <c r="T193" s="20"/>
       <c r="U193" s="20"/>
     </row>
-    <row r="194" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A194" s="7">
         <v>193</v>
       </c>
@@ -11130,7 +11173,7 @@
       <c r="T194" s="20"/>
       <c r="U194" s="20"/>
     </row>
-    <row r="195" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A195" s="7">
         <v>194</v>
       </c>
@@ -11177,7 +11220,7 @@
       <c r="T195" s="20"/>
       <c r="U195" s="20"/>
     </row>
-    <row r="196" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A196" s="7">
         <v>195</v>
       </c>
@@ -11224,7 +11267,7 @@
       <c r="T196" s="20"/>
       <c r="U196" s="20"/>
     </row>
-    <row r="197" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A197" s="7">
         <v>196</v>
       </c>
@@ -11277,7 +11320,7 @@
       <c r="T197" s="20"/>
       <c r="U197" s="20"/>
     </row>
-    <row r="198" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A198" s="7">
         <v>197</v>
       </c>
@@ -11330,7 +11373,7 @@
       <c r="T198" s="20"/>
       <c r="U198" s="20"/>
     </row>
-    <row r="199" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A199" s="7">
         <v>198</v>
       </c>
@@ -11383,7 +11426,7 @@
       <c r="T199" s="20"/>
       <c r="U199" s="20"/>
     </row>
-    <row r="200" spans="1:21" s="44" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" s="44" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A200" s="7">
         <v>199</v>
       </c>
@@ -11436,7 +11479,7 @@
       <c r="T200" s="20"/>
       <c r="U200" s="20"/>
     </row>
-    <row r="201" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="46">
         <v>200</v>
       </c>
@@ -11489,7 +11532,7 @@
       <c r="T201" s="49"/>
       <c r="U201" s="49"/>
     </row>
-    <row r="202" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A202" s="33">
         <v>201</v>
       </c>
@@ -11542,7 +11585,7 @@
       <c r="T202" s="40"/>
       <c r="U202" s="40"/>
     </row>
-    <row r="203" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A203" s="7">
         <v>202</v>
       </c>
@@ -11593,7 +11636,7 @@
       <c r="T203" s="20"/>
       <c r="U203" s="20"/>
     </row>
-    <row r="204" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A204" s="7">
         <v>203</v>
       </c>
@@ -11646,7 +11689,7 @@
       <c r="T204" s="20"/>
       <c r="U204" s="20"/>
     </row>
-    <row r="205" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A205" s="7">
         <v>204</v>
       </c>
@@ -11699,7 +11742,7 @@
       <c r="T205" s="20"/>
       <c r="U205" s="20"/>
     </row>
-    <row r="206" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A206" s="7">
         <v>205</v>
       </c>
@@ -11750,7 +11793,7 @@
       <c r="T206" s="20"/>
       <c r="U206" s="20"/>
     </row>
-    <row r="207" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A207" s="7">
         <v>206</v>
       </c>
@@ -11803,7 +11846,7 @@
       <c r="T207" s="20"/>
       <c r="U207" s="20"/>
     </row>
-    <row r="208" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A208" s="7">
         <v>207</v>
       </c>
@@ -11856,7 +11899,7 @@
       <c r="T208" s="20"/>
       <c r="U208" s="20"/>
     </row>
-    <row r="209" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A209" s="7">
         <v>208</v>
       </c>
@@ -11907,7 +11950,7 @@
       <c r="T209" s="20"/>
       <c r="U209" s="20"/>
     </row>
-    <row r="210" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A210" s="7">
         <v>209</v>
       </c>
@@ -11960,7 +12003,7 @@
       <c r="T210" s="20"/>
       <c r="U210" s="20"/>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="46">
         <v>210</v>
       </c>
@@ -12013,7 +12056,7 @@
       <c r="T211" s="49"/>
       <c r="U211" s="49"/>
     </row>
-    <row r="212" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A212" s="33">
         <v>211</v>
       </c>
@@ -12066,7 +12109,7 @@
       <c r="T212" s="40"/>
       <c r="U212" s="40"/>
     </row>
-    <row r="213" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A213" s="7">
         <v>212</v>
       </c>
@@ -12119,7 +12162,7 @@
       <c r="T213" s="20"/>
       <c r="U213" s="20"/>
     </row>
-    <row r="214" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A214" s="7">
         <v>213</v>
       </c>
@@ -12172,7 +12215,7 @@
       <c r="T214" s="20"/>
       <c r="U214" s="20"/>
     </row>
-    <row r="215" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A215" s="7">
         <v>214</v>
       </c>
@@ -12225,7 +12268,7 @@
       <c r="T215" s="20"/>
       <c r="U215" s="20"/>
     </row>
-    <row r="216" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A216" s="7">
         <v>215</v>
       </c>
@@ -12278,7 +12321,7 @@
       <c r="T216" s="20"/>
       <c r="U216" s="20"/>
     </row>
-    <row r="217" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A217" s="7">
         <v>216</v>
       </c>
@@ -12331,7 +12374,7 @@
       <c r="T217" s="20"/>
       <c r="U217" s="20"/>
     </row>
-    <row r="218" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A218" s="7">
         <v>217</v>
       </c>
@@ -12384,7 +12427,7 @@
       <c r="T218" s="20"/>
       <c r="U218" s="20"/>
     </row>
-    <row r="219" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A219" s="7">
         <v>218</v>
       </c>
@@ -12437,7 +12480,7 @@
       <c r="T219" s="20"/>
       <c r="U219" s="20"/>
     </row>
-    <row r="220" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A220" s="7">
         <v>219</v>
       </c>
@@ -12490,7 +12533,7 @@
       <c r="T220" s="20"/>
       <c r="U220" s="20"/>
     </row>
-    <row r="221" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A221" s="7">
         <v>220</v>
       </c>
@@ -12543,7 +12586,7 @@
       <c r="T221" s="20"/>
       <c r="U221" s="20"/>
     </row>
-    <row r="222" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A222" s="7">
         <v>221</v>
       </c>
@@ -12596,7 +12639,7 @@
       <c r="T222" s="20"/>
       <c r="U222" s="20"/>
     </row>
-    <row r="223" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A223" s="7">
         <v>222</v>
       </c>
@@ -12649,7 +12692,7 @@
       <c r="T223" s="20"/>
       <c r="U223" s="20"/>
     </row>
-    <row r="224" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A224" s="7">
         <v>223</v>
       </c>
@@ -12702,7 +12745,7 @@
       <c r="T224" s="20"/>
       <c r="U224" s="20"/>
     </row>
-    <row r="225" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A225" s="7">
         <v>224</v>
       </c>
@@ -12755,7 +12798,7 @@
       <c r="T225" s="20"/>
       <c r="U225" s="20"/>
     </row>
-    <row r="226" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A226" s="7">
         <v>225</v>
       </c>

</xml_diff>